<commit_message>
vault backup: 2025-12-24 14:50:43
</commit_message>
<xml_diff>
--- a/10-areas/Relationships/Divorce/Applicant (Lenny)/Analysis/CSV/Lenny_Current_Account_with_Joy_Highlighted.xlsx
+++ b/10-areas/Relationships/Divorce/Applicant (Lenny)/Analysis/CSV/Lenny_Current_Account_with_Joy_Highlighted.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CSV Data" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Analysis" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Philippines Analysis" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -55,7 +56,7 @@
       <i val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill/>
     </fill>
@@ -104,6 +105,18 @@
         <bgColor rgb="00FFF2CC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E2EFDA"/>
+        <bgColor rgb="00E2EFDA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FCE4D6"/>
+        <bgColor rgb="00FCE4D6"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -129,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -224,6 +237,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="2" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="6" fillId="10" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -9755,16 +9777,8 @@
           <t>SUMMARY BY CATEGORY</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-    </row>
+    </row>
+    <row r="4"/>
     <row r="5">
       <c r="A5" s="22" t="inlineStr">
         <is>
@@ -9858,12 +9872,7 @@
         <v/>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-    </row>
+    <row r="10"/>
     <row r="11">
       <c r="A11" s="32" t="inlineStr">
         <is>
@@ -10204,6 +10213,931 @@
       <c r="C50" t="inlineStr">
         <is>
           <t>51 transactions</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="70" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="20" t="inlineStr">
+        <is>
+          <t>PHILIPPINES PAYMENTS ANALYSIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="38" t="inlineStr">
+        <is>
+          <t>Analysis of all payments to/from Philippines (including Remitly, PH references, Utang)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>Money Out</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>Money In</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="44" t="inlineStr">
+        <is>
+          <t>2024-08-08</t>
+        </is>
+      </c>
+      <c r="B5" s="44" t="inlineStr">
+        <is>
+          <t>Card Payment to Remitly On 07 Aug</t>
+        </is>
+      </c>
+      <c r="C5" s="45" t="n">
+        <v>30</v>
+      </c>
+      <c r="D5" s="44" t="n"/>
+      <c r="E5" s="44" t="inlineStr">
+        <is>
+          <t>Remitly (Direct)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="44" t="inlineStr">
+        <is>
+          <t>2024-08-19</t>
+        </is>
+      </c>
+      <c r="B6" s="44" t="inlineStr">
+        <is>
+          <t>Card Payment to Remitly On 16 Aug</t>
+        </is>
+      </c>
+      <c r="C6" s="45" t="n">
+        <v>96.81</v>
+      </c>
+      <c r="D6" s="44" t="n"/>
+      <c r="E6" s="44" t="inlineStr">
+        <is>
+          <t>Remitly (Direct)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="44" t="inlineStr">
+        <is>
+          <t>2024-08-20</t>
+        </is>
+      </c>
+      <c r="B7" s="44" t="inlineStr">
+        <is>
+          <t>Card Payment to Remitly On 19 Aug</t>
+        </is>
+      </c>
+      <c r="C7" s="45" t="n">
+        <v>30</v>
+      </c>
+      <c r="D7" s="44" t="n"/>
+      <c r="E7" s="44" t="inlineStr">
+        <is>
+          <t>Remitly (Direct)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="44" t="inlineStr">
+        <is>
+          <t>2024-08-27</t>
+        </is>
+      </c>
+      <c r="B8" s="44" t="inlineStr">
+        <is>
+          <t>Card Payment to Remitly On 25 Aug</t>
+        </is>
+      </c>
+      <c r="C8" s="45" t="n">
+        <v>20</v>
+      </c>
+      <c r="D8" s="44" t="n"/>
+      <c r="E8" s="44" t="inlineStr">
+        <is>
+          <t>Remitly (Direct)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="44" t="inlineStr">
+        <is>
+          <t>2024-08-30</t>
+        </is>
+      </c>
+      <c r="B9" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: PH</t>
+        </is>
+      </c>
+      <c r="C9" s="45" t="n">
+        <v>114</v>
+      </c>
+      <c r="D9" s="44" t="n"/>
+      <c r="E9" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="44" t="inlineStr">
+        <is>
+          <t>2024-08-30</t>
+        </is>
+      </c>
+      <c r="B10" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment From Timog L Ref: Utang</t>
+        </is>
+      </c>
+      <c r="C10" s="44" t="n"/>
+      <c r="D10" s="45" t="n">
+        <v>210</v>
+      </c>
+      <c r="E10" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="44" t="inlineStr">
+        <is>
+          <t>2024-09-05</t>
+        </is>
+      </c>
+      <c r="B11" s="44" t="inlineStr">
+        <is>
+          <t>Card Payment to Remitly On 04 Sep</t>
+        </is>
+      </c>
+      <c r="C11" s="45" t="n">
+        <v>20</v>
+      </c>
+      <c r="D11" s="44" t="n"/>
+      <c r="E11" s="44" t="inlineStr">
+        <is>
+          <t>Remitly (Direct)</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="44" t="inlineStr">
+        <is>
+          <t>2024-09-06</t>
+        </is>
+      </c>
+      <c r="B12" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Joylyn Gray Ref: PH - Bags</t>
+        </is>
+      </c>
+      <c r="C12" s="45" t="n">
+        <v>95</v>
+      </c>
+      <c r="D12" s="44" t="n"/>
+      <c r="E12" s="44" t="inlineStr">
+        <is>
+          <t>Via Joylyn Gray</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="44" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="B13" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Remitly UK Ref: 12250080062</t>
+        </is>
+      </c>
+      <c r="C13" s="45" t="n">
+        <v>130</v>
+      </c>
+      <c r="D13" s="44" t="n"/>
+      <c r="E13" s="44" t="inlineStr">
+        <is>
+          <t>Remitly (Direct)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="44" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="B14" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: PH Budget</t>
+        </is>
+      </c>
+      <c r="C14" s="45" t="n">
+        <v>235</v>
+      </c>
+      <c r="D14" s="44" t="n"/>
+      <c r="E14" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="44" t="inlineStr">
+        <is>
+          <t>2024-10-21</t>
+        </is>
+      </c>
+      <c r="B15" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Remitly UK Ref: 12290052587</t>
+        </is>
+      </c>
+      <c r="C15" s="45" t="n">
+        <v>66</v>
+      </c>
+      <c r="D15" s="44" t="n"/>
+      <c r="E15" s="44" t="inlineStr">
+        <is>
+          <t>Remitly (Direct)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="44" t="inlineStr">
+        <is>
+          <t>2024-10-21</t>
+        </is>
+      </c>
+      <c r="B16" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Joylyn Gray Ref: PH Xmas Decors</t>
+        </is>
+      </c>
+      <c r="C16" s="45" t="n">
+        <v>26</v>
+      </c>
+      <c r="D16" s="44" t="n"/>
+      <c r="E16" s="44" t="inlineStr">
+        <is>
+          <t>Via Joylyn Gray</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="44" t="inlineStr">
+        <is>
+          <t>2024-10-22</t>
+        </is>
+      </c>
+      <c r="B17" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Joylyn Gray Ref: PH</t>
+        </is>
+      </c>
+      <c r="C17" s="45" t="n">
+        <v>181</v>
+      </c>
+      <c r="D17" s="44" t="n"/>
+      <c r="E17" s="44" t="inlineStr">
+        <is>
+          <t>Via Joylyn Gray</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="44" t="inlineStr">
+        <is>
+          <t>2024-10-22</t>
+        </is>
+      </c>
+      <c r="B18" s="44" t="inlineStr">
+        <is>
+          <t>Transfer From Sort Code 20-05-57 Account 23827119 Ref: PH</t>
+        </is>
+      </c>
+      <c r="C18" s="44" t="n"/>
+      <c r="D18" s="45" t="n">
+        <v>181</v>
+      </c>
+      <c r="E18" s="44" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="44" t="inlineStr">
+        <is>
+          <t>2024-10-31</t>
+        </is>
+      </c>
+      <c r="B19" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: PH Budget</t>
+        </is>
+      </c>
+      <c r="C19" s="45" t="n">
+        <v>254</v>
+      </c>
+      <c r="D19" s="44" t="n"/>
+      <c r="E19" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="44" t="inlineStr">
+        <is>
+          <t>2025-01-31</t>
+        </is>
+      </c>
+      <c r="B20" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: PH Feb</t>
+        </is>
+      </c>
+      <c r="C20" s="45" t="n">
+        <v>238</v>
+      </c>
+      <c r="D20" s="44" t="n"/>
+      <c r="E20" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="44" t="inlineStr">
+        <is>
+          <t>2025-02-28</t>
+        </is>
+      </c>
+      <c r="B21" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Joylyn Gray Ref: PH</t>
+        </is>
+      </c>
+      <c r="C21" s="45" t="n">
+        <v>269</v>
+      </c>
+      <c r="D21" s="44" t="n"/>
+      <c r="E21" s="44" t="inlineStr">
+        <is>
+          <t>Via Joylyn Gray</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="44" t="inlineStr">
+        <is>
+          <t>2025-02-28</t>
+        </is>
+      </c>
+      <c r="B22" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: PH</t>
+        </is>
+      </c>
+      <c r="C22" s="45" t="n">
+        <v>269</v>
+      </c>
+      <c r="D22" s="44" t="n"/>
+      <c r="E22" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="44" t="inlineStr">
+        <is>
+          <t>2025-04-07</t>
+        </is>
+      </c>
+      <c r="B23" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: PH Budget</t>
+        </is>
+      </c>
+      <c r="C23" s="45" t="n">
+        <v>436</v>
+      </c>
+      <c r="D23" s="44" t="n"/>
+      <c r="E23" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="44" t="inlineStr">
+        <is>
+          <t>2025-04-30</t>
+        </is>
+      </c>
+      <c r="B24" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: PH</t>
+        </is>
+      </c>
+      <c r="C24" s="45" t="n">
+        <v>135</v>
+      </c>
+      <c r="D24" s="44" t="n"/>
+      <c r="E24" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="44" t="inlineStr">
+        <is>
+          <t>2025-05-13</t>
+        </is>
+      </c>
+      <c r="B25" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: PH</t>
+        </is>
+      </c>
+      <c r="C25" s="45" t="n">
+        <v>50</v>
+      </c>
+      <c r="D25" s="44" t="n"/>
+      <c r="E25" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="44" t="inlineStr">
+        <is>
+          <t>2025-05-30</t>
+        </is>
+      </c>
+      <c r="B26" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: PH</t>
+        </is>
+      </c>
+      <c r="C26" s="45" t="n">
+        <v>146</v>
+      </c>
+      <c r="D26" s="44" t="n"/>
+      <c r="E26" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="44" t="inlineStr">
+        <is>
+          <t>2025-06-30</t>
+        </is>
+      </c>
+      <c r="B27" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: PH</t>
+        </is>
+      </c>
+      <c r="C27" s="45" t="n">
+        <v>152</v>
+      </c>
+      <c r="D27" s="44" t="n"/>
+      <c r="E27" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="44" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+      <c r="B28" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: PH</t>
+        </is>
+      </c>
+      <c r="C28" s="45" t="n">
+        <v>50</v>
+      </c>
+      <c r="D28" s="44" t="n"/>
+      <c r="E28" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="44" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+      <c r="B29" s="44" t="inlineStr">
+        <is>
+          <t>Transfer From Sort Code 20-05-57 Account 23827119 Ref: PH</t>
+        </is>
+      </c>
+      <c r="C29" s="44" t="n"/>
+      <c r="D29" s="45" t="n">
+        <v>50</v>
+      </c>
+      <c r="E29" s="44" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="44" t="inlineStr">
+        <is>
+          <t>2025-08-13</t>
+        </is>
+      </c>
+      <c r="B30" s="44" t="inlineStr">
+        <is>
+          <t>Card Payment to Remitly On 12 Aug</t>
+        </is>
+      </c>
+      <c r="C30" s="45" t="n">
+        <v>331.99</v>
+      </c>
+      <c r="D30" s="44" t="n"/>
+      <c r="E30" s="44" t="inlineStr">
+        <is>
+          <t>Remitly (Direct)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="44" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B31" s="44" t="inlineStr">
+        <is>
+          <t>Card Payment to Remitly On 20 Aug</t>
+        </is>
+      </c>
+      <c r="C31" s="45" t="n">
+        <v>151.99</v>
+      </c>
+      <c r="D31" s="44" t="n"/>
+      <c r="E31" s="44" t="inlineStr">
+        <is>
+          <t>Remitly (Direct)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="44" t="inlineStr">
+        <is>
+          <t>2025-09-01</t>
+        </is>
+      </c>
+      <c r="B32" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: PH</t>
+        </is>
+      </c>
+      <c r="C32" s="45" t="n">
+        <v>130</v>
+      </c>
+      <c r="D32" s="44" t="n"/>
+      <c r="E32" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="44" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="B33" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: Utang</t>
+        </is>
+      </c>
+      <c r="C33" s="45" t="n">
+        <v>50</v>
+      </c>
+      <c r="D33" s="44" t="n"/>
+      <c r="E33" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="44" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B34" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: PH Budget</t>
+        </is>
+      </c>
+      <c r="C34" s="45" t="n">
+        <v>129</v>
+      </c>
+      <c r="D34" s="44" t="n"/>
+      <c r="E34" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="44" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B35" s="44" t="inlineStr">
+        <is>
+          <t>Bill Payment to Lucy Timog Ref: PH</t>
+        </is>
+      </c>
+      <c r="C35" s="45" t="n">
+        <v>130</v>
+      </c>
+      <c r="D35" s="44" t="n"/>
+      <c r="E35" s="44" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="21" t="inlineStr">
+        <is>
+          <t>SUMMARY BY CATEGORY</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="46" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="B40" s="46" t="inlineStr">
+        <is>
+          <t>Net Amount</t>
+        </is>
+      </c>
+      <c r="C40" s="46" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="47" t="inlineStr">
+        <is>
+          <t>Remitly (Direct Transfers)</t>
+        </is>
+      </c>
+      <c r="B41" s="48" t="n">
+        <v>876.79</v>
+      </c>
+      <c r="C41" s="47" t="inlineStr">
+        <is>
+          <t>Direct payments via Remitly service to Philippines</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="47" t="inlineStr">
+        <is>
+          <t>Via Joylyn Gray</t>
+        </is>
+      </c>
+      <c r="B42" s="48" t="n">
+        <v>571</v>
+      </c>
+      <c r="C42" s="47" t="inlineStr">
+        <is>
+          <t>Payments to Joy marked 'PH'</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="47" t="inlineStr">
+        <is>
+          <t>Via Lucy Timog</t>
+        </is>
+      </c>
+      <c r="B43" s="48" t="n">
+        <v>2308</v>
+      </c>
+      <c r="C43" s="47" t="inlineStr">
+        <is>
+          <t>Payments to Lucy marked 'PH' or 'PH Budget'</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="47" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="B44" s="48" t="n">
+        <v>-231</v>
+      </c>
+      <c r="C44" s="47" t="inlineStr">
+        <is>
+          <t>Misc PH-related transfers</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="47" t="inlineStr"/>
+      <c r="B45" s="47" t="inlineStr"/>
+      <c r="C45" s="47" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="49" t="inlineStr">
+        <is>
+          <t>TOTAL NET OUT TO PHILIPPINES</t>
+        </is>
+      </c>
+      <c r="B46" s="50" t="n">
+        <v>3524.79</v>
+      </c>
+      <c r="C46" s="49" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="34" t="inlineStr">
+        <is>
+          <t>KEY FINDINGS:</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="38" t="inlineStr">
+        <is>
+          <t>• Total net outflow to Philippines: £3,524.79</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="38" t="inlineStr">
+        <is>
+          <t>• Period covered: August 2024 - October 2025 (15 months)</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="38" t="inlineStr">
+        <is>
+          <t>• Average monthly outflow: £234.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="34" t="inlineStr">
+        <is>
+          <t>PATTERN ANALYSIS:</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="38" t="inlineStr">
+        <is>
+          <t>• Large payments via Lucy Timog labeled 'PH Budget' suggest regular remittances</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="38" t="inlineStr">
+        <is>
+          <t>• Some payments labeled 'Utang' (Tagalog for 'debt')</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="38" t="inlineStr">
+        <is>
+          <t>• Feb 2024: Lenny informed Mark she was purchasing land in Philippines</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="38" t="inlineStr">
+        <is>
+          <t>• Form E Section 2.10 (Foreign property): No disclosure of Philippines property</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="34" t="inlineStr">
+        <is>
+          <t>QUESTIONS ARISING:</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="38" t="inlineStr">
+        <is>
+          <t>1. Are these payments family remittances to parents?</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="38" t="inlineStr">
+        <is>
+          <t>2. Are these payments for purchase of land/property in Philippines?</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="38" t="inlineStr">
+        <is>
+          <t>3. If property purchased, why not disclosed in Form E?</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="38" t="inlineStr">
+        <is>
+          <t>4. What is current value of any Philippines property owned?</t>
         </is>
       </c>
     </row>

</xml_diff>